<commit_message>
MySQL migration adjustment continuation
</commit_message>
<xml_diff>
--- a/other files/2014 OP FOR DBASE.xlsx
+++ b/other files/2014 OP FOR DBASE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\django project\nafd_v2_0.5\other files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\nafd\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="125">
   <si>
     <t>SUF=Rate(SUF) x BW x 1000</t>
   </si>
@@ -382,6 +382,18 @@
   </si>
   <si>
     <t>EXPIRY DATE:</t>
+  </si>
+  <si>
+    <t>Site No</t>
+  </si>
+  <si>
+    <t>site_no</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>city</t>
   </si>
 </sst>
 </file>
@@ -533,7 +545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1048,6 +1060,17 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1058,7 +1081,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1211,28 +1234,250 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1244,222 +1489,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1767,383 +1811,399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV127"/>
+  <dimension ref="A1:AX127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51:C51"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" customWidth="1"/>
-    <col min="14" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" customWidth="1"/>
-    <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="18" width="5.7109375" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" customWidth="1"/>
-    <col min="20" max="21" width="4.42578125" customWidth="1"/>
-    <col min="22" max="22" width="6.5703125" customWidth="1"/>
-    <col min="23" max="23" width="5.28515625" customWidth="1"/>
-    <col min="24" max="24" width="4.7109375" customWidth="1"/>
-    <col min="25" max="25" width="7.85546875" customWidth="1"/>
-    <col min="26" max="26" width="8.5703125" customWidth="1"/>
-    <col min="27" max="27" width="7.5703125" customWidth="1"/>
-    <col min="28" max="28" width="4.28515625" customWidth="1"/>
-    <col min="29" max="29" width="5.5703125" customWidth="1"/>
-    <col min="30" max="30" width="5.42578125" customWidth="1"/>
-    <col min="31" max="31" width="4.140625" customWidth="1"/>
-    <col min="32" max="32" width="6" customWidth="1"/>
-    <col min="33" max="33" width="3.42578125" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" customWidth="1"/>
-    <col min="35" max="35" width="4.5703125" customWidth="1"/>
-    <col min="36" max="36" width="5.7109375" customWidth="1"/>
-    <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="70" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" customWidth="1"/>
+    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" customWidth="1"/>
+    <col min="16" max="16" width="8" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" customWidth="1"/>
+    <col min="19" max="19" width="5" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" customWidth="1"/>
+    <col min="22" max="23" width="4.42578125" customWidth="1"/>
+    <col min="24" max="24" width="6.5703125" customWidth="1"/>
+    <col min="25" max="25" width="5.28515625" customWidth="1"/>
+    <col min="26" max="26" width="4.7109375" customWidth="1"/>
+    <col min="27" max="27" width="7.85546875" customWidth="1"/>
+    <col min="28" max="28" width="8.5703125" customWidth="1"/>
+    <col min="29" max="29" width="7.5703125" customWidth="1"/>
+    <col min="30" max="30" width="4.28515625" customWidth="1"/>
+    <col min="31" max="31" width="5.5703125" customWidth="1"/>
+    <col min="32" max="32" width="5.42578125" customWidth="1"/>
+    <col min="33" max="33" width="4.140625" customWidth="1"/>
+    <col min="34" max="34" width="6" customWidth="1"/>
+    <col min="35" max="35" width="3.42578125" customWidth="1"/>
+    <col min="36" max="36" width="6.140625" customWidth="1"/>
+    <col min="37" max="37" width="4.5703125" customWidth="1"/>
+    <col min="38" max="38" width="5.7109375" customWidth="1"/>
+    <col min="39" max="40" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+    <row r="1" spans="1:50" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="116"/>
-      <c r="R1" s="116"/>
-      <c r="S1" s="116"/>
-      <c r="T1" s="116"/>
-      <c r="U1" s="116"/>
-      <c r="V1" s="116"/>
-      <c r="W1" s="116"/>
-      <c r="X1" s="116"/>
-      <c r="Y1" s="116"/>
-      <c r="Z1" s="116"/>
-      <c r="AA1" s="116"/>
-      <c r="AB1" s="116"/>
-      <c r="AC1" s="116"/>
-      <c r="AD1" s="116"/>
-      <c r="AE1" s="116"/>
-      <c r="AF1" s="116"/>
-      <c r="AG1" s="116"/>
-      <c r="AH1" s="116"/>
-      <c r="AI1" s="116"/>
-      <c r="AJ1" s="116"/>
-    </row>
-    <row r="2" spans="1:48" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="113"/>
+      <c r="AA1" s="113"/>
+      <c r="AB1" s="113"/>
+      <c r="AC1" s="113"/>
+      <c r="AD1" s="113"/>
+      <c r="AE1" s="113"/>
+      <c r="AF1" s="113"/>
+      <c r="AG1" s="113"/>
+      <c r="AH1" s="113"/>
+      <c r="AI1" s="113"/>
+      <c r="AJ1" s="113"/>
+      <c r="AK1" s="113"/>
+      <c r="AL1" s="113"/>
+    </row>
+    <row r="2" spans="1:50" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="120"/>
-      <c r="Z2" s="120"/>
-      <c r="AA2" s="120"/>
-      <c r="AB2" s="120"/>
-      <c r="AC2" s="120"/>
-      <c r="AD2" s="120"/>
-      <c r="AE2" s="120"/>
-      <c r="AF2" s="120"/>
-      <c r="AG2" s="120"/>
-      <c r="AH2" s="120"/>
-      <c r="AI2" s="120"/>
-      <c r="AJ2" s="120"/>
-    </row>
-    <row r="3" spans="1:48" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A3" s="116" t="s">
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
+      <c r="P2" s="119"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="119"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
+      <c r="Y2" s="119"/>
+      <c r="Z2" s="119"/>
+      <c r="AA2" s="119"/>
+      <c r="AB2" s="119"/>
+      <c r="AC2" s="119"/>
+      <c r="AD2" s="119"/>
+      <c r="AE2" s="119"/>
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="119"/>
+      <c r="AH2" s="119"/>
+      <c r="AI2" s="119"/>
+      <c r="AJ2" s="119"/>
+      <c r="AK2" s="119"/>
+      <c r="AL2" s="119"/>
+    </row>
+    <row r="3" spans="1:50" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A3" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
-      <c r="R3" s="116"/>
-      <c r="S3" s="116"/>
-      <c r="T3" s="116"/>
-      <c r="U3" s="116"/>
-      <c r="V3" s="116"/>
-      <c r="W3" s="116"/>
-      <c r="X3" s="116"/>
-      <c r="Y3" s="116"/>
-      <c r="Z3" s="116"/>
-      <c r="AA3" s="116"/>
-      <c r="AB3" s="116"/>
-      <c r="AC3" s="116"/>
-      <c r="AD3" s="116"/>
-      <c r="AE3" s="116"/>
-      <c r="AF3" s="116"/>
-      <c r="AG3" s="116"/>
-      <c r="AH3" s="116"/>
-      <c r="AI3" s="116"/>
-      <c r="AJ3" s="116"/>
-    </row>
-    <row r="4" spans="1:48" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="113"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
+      <c r="Q3" s="113"/>
+      <c r="R3" s="113"/>
+      <c r="S3" s="113"/>
+      <c r="T3" s="113"/>
+      <c r="U3" s="113"/>
+      <c r="V3" s="113"/>
+      <c r="W3" s="113"/>
+      <c r="X3" s="113"/>
+      <c r="Y3" s="113"/>
+      <c r="Z3" s="113"/>
+      <c r="AA3" s="113"/>
+      <c r="AB3" s="113"/>
+      <c r="AC3" s="113"/>
+      <c r="AD3" s="113"/>
+      <c r="AE3" s="113"/>
+      <c r="AF3" s="113"/>
+      <c r="AG3" s="113"/>
+      <c r="AH3" s="113"/>
+      <c r="AI3" s="113"/>
+      <c r="AJ3" s="113"/>
+      <c r="AK3" s="113"/>
+      <c r="AL3" s="113"/>
+    </row>
+    <row r="4" spans="1:50" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="68"/>
-    </row>
-    <row r="5" spans="1:48" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="68"/>
+    </row>
+    <row r="5" spans="1:50" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-    </row>
-    <row r="6" spans="1:48" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+    </row>
+    <row r="6" spans="1:50" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="19"/>
-      <c r="C6" s="2"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="99" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="19"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="99" t="s">
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="133"/>
+      <c r="U6" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="T6" s="110"/>
-      <c r="U6" s="110"/>
-      <c r="V6" s="110"/>
-      <c r="W6" s="110"/>
-      <c r="X6" s="110"/>
-      <c r="Y6" s="111"/>
-      <c r="AB6" s="107" t="s">
+      <c r="V6" s="138"/>
+      <c r="W6" s="138"/>
+      <c r="X6" s="138"/>
+      <c r="Y6" s="138"/>
+      <c r="Z6" s="138"/>
+      <c r="AA6" s="139"/>
+      <c r="AD6" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="AC6" s="108"/>
-      <c r="AD6" s="109"/>
-      <c r="AE6" s="107" t="s">
+      <c r="AE6" s="123"/>
+      <c r="AF6" s="124"/>
+      <c r="AG6" s="122" t="s">
         <v>65</v>
       </c>
-      <c r="AF6" s="108"/>
-      <c r="AG6" s="108"/>
-      <c r="AH6" s="109"/>
-    </row>
-    <row r="7" spans="1:48" s="3" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH6" s="123"/>
+      <c r="AI6" s="123"/>
+      <c r="AJ6" s="124"/>
+    </row>
+    <row r="7" spans="1:50" s="3" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="8"/>
       <c r="E7" s="37"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="117" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="93" t="s">
+      <c r="K7" s="115"/>
+      <c r="L7" s="115"/>
+      <c r="M7" s="116"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="117" t="s">
         <v>114</v>
       </c>
-      <c r="N7" s="106"/>
-      <c r="O7" s="93" t="s">
+      <c r="P7" s="118"/>
+      <c r="Q7" s="117" t="s">
         <v>115</v>
       </c>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="93" t="s">
+      <c r="R7" s="118"/>
+      <c r="S7" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="R7" s="106"/>
-      <c r="S7" s="102" t="s">
+      <c r="T7" s="118"/>
+      <c r="U7" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="104" t="s">
+      <c r="V7" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="93" t="s">
+      <c r="W7" s="117" t="s">
         <v>117</v>
       </c>
-      <c r="V7" s="106"/>
-      <c r="W7" s="93" t="s">
+      <c r="X7" s="118"/>
+      <c r="Y7" s="117" t="s">
         <v>118</v>
       </c>
-      <c r="X7" s="106"/>
-      <c r="Y7" s="93" t="s">
+      <c r="Z7" s="118"/>
+      <c r="AA7" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="Z7" s="94"/>
-      <c r="AA7" s="97" t="s">
+      <c r="AB7" s="126"/>
+      <c r="AC7" s="129" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="95" t="s">
+      <c r="AD7" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="AC7" s="93" t="s">
+      <c r="AE7" s="117" t="s">
         <v>119</v>
       </c>
-      <c r="AD7" s="106"/>
-      <c r="AE7" s="93" t="s">
+      <c r="AF7" s="118"/>
+      <c r="AG7" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="AF7" s="106"/>
-      <c r="AG7" s="93" t="s">
+      <c r="AH7" s="118"/>
+      <c r="AI7" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="AH7" s="106"/>
-      <c r="AI7" s="93" t="s">
+      <c r="AJ7" s="118"/>
+      <c r="AK7" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="AJ7" s="106"/>
-    </row>
-    <row r="8" spans="1:48" s="3" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AL7" s="118"/>
+    </row>
+    <row r="8" spans="1:50" s="3" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="D8" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="G8" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="H8" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="I8" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="J8" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="K8" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="L8" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="40" t="s">
+      <c r="M8" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="N8" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="M8" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>8</v>
       </c>
       <c r="O8" s="43" t="s">
         <v>62</v>
       </c>
       <c r="P8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="43" t="s">
+      <c r="S8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="R8" s="16" t="s">
+      <c r="T8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="S8" s="103"/>
-      <c r="T8" s="105"/>
-      <c r="U8" s="51" t="s">
+      <c r="U8" s="135"/>
+      <c r="V8" s="137"/>
+      <c r="W8" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="V8" s="52" t="s">
+      <c r="X8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="W8" s="51" t="s">
+      <c r="Y8" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="X8" s="52" t="s">
+      <c r="Z8" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="Y8" s="45" t="s">
+      <c r="AA8" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="Z8" s="46" t="s">
+      <c r="AB8" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="AA8" s="98"/>
-      <c r="AB8" s="96"/>
-      <c r="AC8" s="43" t="s">
+      <c r="AC8" s="130"/>
+      <c r="AD8" s="128"/>
+      <c r="AE8" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="AD8" s="16" t="s">
+      <c r="AF8" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="AE8" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF8" s="16" t="s">
-        <v>12</v>
       </c>
       <c r="AG8" s="43" t="s">
         <v>60</v>
@@ -2152,2198 +2212,2348 @@
         <v>12</v>
       </c>
       <c r="AI8" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK8" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="AJ8" s="16" t="s">
+      <c r="AL8" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:48" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:50" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="13"/>
-      <c r="C9" s="7"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="L9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="44"/>
+      <c r="M9" s="11"/>
       <c r="N9" s="17"/>
       <c r="O9" s="44"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="44"/>
       <c r="R9" s="17"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="17"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="7"/>
       <c r="W9" s="44"/>
       <c r="X9" s="17"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="48"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="44"/>
-      <c r="AD9" s="17"/>
+      <c r="Y9" s="44"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="47"/>
+      <c r="AB9" s="48"/>
+      <c r="AC9" s="55"/>
+      <c r="AD9" s="7"/>
       <c r="AE9" s="44"/>
       <c r="AF9" s="17"/>
       <c r="AG9" s="44"/>
       <c r="AH9" s="17"/>
       <c r="AI9" s="44"/>
       <c r="AJ9" s="17"/>
-    </row>
-    <row r="10" spans="1:48" s="67" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="AK9" s="44"/>
+      <c r="AL9" s="17"/>
+    </row>
+    <row r="10" spans="1:50" s="67" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="D10" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="E10" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="G10" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="H10" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="63" t="s">
+      <c r="I10" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="63" t="s">
+      <c r="J10" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="63" t="s">
+      <c r="K10" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="J10" s="63" t="s">
+      <c r="L10" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="63" t="s">
+      <c r="M10" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="63" t="s">
+      <c r="N10" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="M10" s="63" t="s">
+      <c r="O10" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="N10" s="63" t="s">
+      <c r="P10" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="O10" s="63" t="s">
+      <c r="Q10" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="P10" s="63" t="s">
+      <c r="R10" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="Q10" s="65" t="s">
+      <c r="S10" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="R10" s="65" t="s">
+      <c r="T10" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="S10" s="64" t="s">
+      <c r="U10" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="T10" s="64" t="s">
+      <c r="V10" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="U10" s="65" t="s">
+      <c r="W10" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="V10" s="65" t="s">
+      <c r="X10" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="W10" s="65" t="s">
+      <c r="Y10" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="X10" s="65" t="s">
+      <c r="Z10" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="Y10" s="65" t="s">
+      <c r="AA10" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="Z10" s="63" t="s">
+      <c r="AB10" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="AA10" s="63" t="s">
+      <c r="AC10" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="AB10" s="63" t="s">
+      <c r="AD10" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="AC10" s="63" t="s">
+      <c r="AE10" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="AD10" s="63" t="s">
+      <c r="AF10" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="AE10" s="63" t="s">
+      <c r="AG10" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="AF10" s="63" t="s">
+      <c r="AH10" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="AG10" s="63" t="s">
+      <c r="AI10" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="AH10" s="63" t="s">
+      <c r="AJ10" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="AI10" s="63" t="s">
+      <c r="AK10" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="AJ10" s="63" t="s">
+      <c r="AL10" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="AK10" s="63"/>
-      <c r="AL10" s="63"/>
       <c r="AM10" s="63"/>
-      <c r="AN10" s="65"/>
-      <c r="AO10" s="65"/>
-      <c r="AP10" s="63"/>
-      <c r="AQ10" s="63"/>
+      <c r="AN10" s="63"/>
+      <c r="AO10" s="63"/>
+      <c r="AP10" s="65"/>
+      <c r="AQ10" s="65"/>
       <c r="AR10" s="63"/>
       <c r="AS10" s="63"/>
       <c r="AT10" s="63"/>
       <c r="AU10" s="63"/>
-      <c r="AV10" s="66"/>
-    </row>
-    <row r="11" spans="1:48" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="121">
+      <c r="AV10" s="63"/>
+      <c r="AW10" s="63"/>
+      <c r="AX10" s="66"/>
+    </row>
+    <row r="11" spans="1:50" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="71">
         <v>1</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="164"/>
+      <c r="C11" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="123"/>
-      <c r="D11" s="124"/>
-      <c r="E11" s="124">
+      <c r="D11" s="73"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74">
         <v>2</v>
       </c>
-      <c r="F11" s="124">
+      <c r="H11" s="74">
         <v>1</v>
       </c>
-      <c r="G11" s="125">
+      <c r="I11" s="75">
         <v>1</v>
       </c>
-      <c r="H11" s="126">
+      <c r="J11" s="76">
         <v>2</v>
       </c>
-      <c r="I11" s="124">
+      <c r="K11" s="74">
         <v>7</v>
       </c>
-      <c r="J11" s="124">
+      <c r="L11" s="74">
         <v>27.5</v>
       </c>
-      <c r="K11" s="127">
-        <f>J11*H11*G11*1000</f>
+      <c r="M11" s="77">
+        <f>L11*J11*I11*1000</f>
         <v>55000</v>
       </c>
-      <c r="L11" s="128">
-        <f>K11*E11</f>
+      <c r="N11" s="78">
+        <f>M11*G11</f>
         <v>110000</v>
       </c>
-      <c r="M11" s="125">
+      <c r="O11" s="75">
         <v>480</v>
       </c>
-      <c r="N11" s="129">
-        <f>G11*M11*E11</f>
+      <c r="P11" s="79">
+        <f>I11*O11*G11</f>
         <v>960</v>
       </c>
-      <c r="O11" s="125">
+      <c r="Q11" s="75">
         <v>480</v>
       </c>
-      <c r="P11" s="129">
-        <f>G11*O11*E11</f>
+      <c r="R11" s="79">
+        <f>I11*Q11*G11</f>
         <v>960</v>
       </c>
-      <c r="Q11" s="125"/>
-      <c r="R11" s="129">
-        <f>G11*Q11</f>
+      <c r="S11" s="75"/>
+      <c r="T11" s="79">
+        <f>I11*S11</f>
         <v>0</v>
       </c>
-      <c r="S11" s="130">
+      <c r="U11" s="80">
         <v>1</v>
       </c>
-      <c r="T11" s="124">
+      <c r="V11" s="74">
         <v>1</v>
       </c>
-      <c r="U11" s="125">
+      <c r="W11" s="75">
         <v>96</v>
       </c>
-      <c r="V11" s="129">
-        <f>T11*U11*S11</f>
+      <c r="X11" s="79">
+        <f>V11*W11*U11</f>
         <v>96</v>
       </c>
-      <c r="W11" s="125">
+      <c r="Y11" s="75">
         <v>60</v>
       </c>
-      <c r="X11" s="129">
-        <f t="shared" ref="X11" si="0">W11*T11</f>
+      <c r="Z11" s="79">
+        <f t="shared" ref="Z11" si="0">Y11*V11</f>
         <v>60</v>
       </c>
-      <c r="Y11" s="131">
-        <f t="shared" ref="Y11:Y12" si="1">180*T11</f>
+      <c r="AA11" s="81">
+        <f t="shared" ref="AA11:AA12" si="1">180*V11</f>
         <v>180</v>
       </c>
-      <c r="Z11" s="132">
+      <c r="AB11" s="82">
         <v>180</v>
       </c>
-      <c r="AA11" s="133">
+      <c r="AC11" s="83">
         <v>180</v>
       </c>
-      <c r="AB11" s="124">
+      <c r="AD11" s="74">
         <v>1</v>
       </c>
-      <c r="AC11" s="125">
+      <c r="AE11" s="75">
         <v>60</v>
       </c>
-      <c r="AD11" s="129">
-        <f t="shared" ref="AD11:AD12" si="2">AC11*AB11</f>
+      <c r="AF11" s="79">
+        <f t="shared" ref="AF11:AF12" si="2">AE11*AD11</f>
         <v>60</v>
       </c>
-      <c r="AE11" s="134"/>
-      <c r="AF11" s="128">
-        <f>AE11*N11</f>
+      <c r="AG11" s="84"/>
+      <c r="AH11" s="78">
+        <f>AG11*P11</f>
         <v>0</v>
       </c>
-      <c r="AG11" s="134"/>
-      <c r="AH11" s="128">
-        <f>AG11*K11</f>
+      <c r="AI11" s="84"/>
+      <c r="AJ11" s="78">
+        <f>AI11*M11</f>
         <v>0</v>
       </c>
-      <c r="AI11" s="135"/>
-      <c r="AJ11" s="129">
+      <c r="AK11" s="85"/>
+      <c r="AL11" s="79">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:48" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="121">
+    <row r="12" spans="1:50" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="71">
         <v>2</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="164"/>
+      <c r="C12" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="123" t="s">
+      <c r="D12" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="124"/>
-      <c r="E12" s="124">
+      <c r="E12" s="167"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74">
         <v>2</v>
       </c>
-      <c r="F12" s="124">
+      <c r="H12" s="74">
         <v>2</v>
       </c>
-      <c r="G12" s="125">
+      <c r="I12" s="75">
         <v>1</v>
       </c>
-      <c r="H12" s="126">
+      <c r="J12" s="76">
         <v>2</v>
       </c>
-      <c r="I12" s="124">
+      <c r="K12" s="74">
         <v>7</v>
       </c>
-      <c r="J12" s="124">
+      <c r="L12" s="74">
         <v>27.5</v>
       </c>
-      <c r="K12" s="127">
-        <f>J12*H12*G12*1000</f>
+      <c r="M12" s="77">
+        <f>L12*J12*I12*1000</f>
         <v>55000</v>
       </c>
-      <c r="L12" s="128">
-        <f>K12*E12</f>
+      <c r="N12" s="78">
+        <f>M12*G12</f>
         <v>110000</v>
       </c>
-      <c r="M12" s="125">
+      <c r="O12" s="75">
         <v>480</v>
       </c>
-      <c r="N12" s="129">
-        <f>G12*M12*E12</f>
+      <c r="P12" s="79">
+        <f>I12*O12*G12</f>
         <v>960</v>
       </c>
-      <c r="O12" s="125">
+      <c r="Q12" s="75">
         <v>480</v>
       </c>
-      <c r="P12" s="129">
-        <f>G12*O12*E12</f>
+      <c r="R12" s="79">
+        <f>I12*Q12*G12</f>
         <v>960</v>
       </c>
-      <c r="Q12" s="125"/>
-      <c r="R12" s="129">
-        <f>G12*Q12</f>
+      <c r="S12" s="75"/>
+      <c r="T12" s="79">
+        <f>I12*S12</f>
         <v>0</v>
       </c>
-      <c r="S12" s="130">
+      <c r="U12" s="80">
         <v>1</v>
       </c>
-      <c r="T12" s="124">
+      <c r="V12" s="74">
         <v>1</v>
       </c>
-      <c r="U12" s="125">
+      <c r="W12" s="75">
         <v>96</v>
       </c>
-      <c r="V12" s="129">
-        <f>T12*U12*S12</f>
+      <c r="X12" s="79">
+        <f>V12*W12*U12</f>
         <v>96</v>
       </c>
-      <c r="W12" s="125">
+      <c r="Y12" s="75">
         <v>60</v>
       </c>
-      <c r="X12" s="129">
-        <f t="shared" ref="X12:X15" si="3">W12*T12</f>
+      <c r="Z12" s="79">
+        <f t="shared" ref="Z12:Z15" si="3">Y12*V12</f>
         <v>60</v>
       </c>
-      <c r="Y12" s="131">
+      <c r="AA12" s="81">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="Z12" s="132">
+      <c r="AB12" s="82">
         <v>180</v>
       </c>
-      <c r="AA12" s="133">
+      <c r="AC12" s="83">
         <v>180</v>
       </c>
-      <c r="AB12" s="124">
+      <c r="AD12" s="74">
         <v>1</v>
       </c>
-      <c r="AC12" s="125">
+      <c r="AE12" s="75">
         <v>60</v>
       </c>
-      <c r="AD12" s="129">
+      <c r="AF12" s="79">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="AE12" s="134"/>
-      <c r="AF12" s="128">
-        <f>AE12*N12</f>
+      <c r="AG12" s="84"/>
+      <c r="AH12" s="78">
+        <f>AG12*P12</f>
         <v>0</v>
       </c>
-      <c r="AG12" s="134"/>
-      <c r="AH12" s="128">
-        <f>AG12*K12</f>
+      <c r="AI12" s="84"/>
+      <c r="AJ12" s="78">
+        <f>AI12*M12</f>
         <v>0</v>
       </c>
-      <c r="AI12" s="135"/>
-      <c r="AJ12" s="129">
+      <c r="AK12" s="85"/>
+      <c r="AL12" s="79">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:48" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="121"/>
-      <c r="B13" s="122"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="124"/>
-      <c r="E13" s="124">
+    <row r="13" spans="1:50" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="71"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74">
         <v>2</v>
       </c>
-      <c r="F13" s="124"/>
-      <c r="G13" s="137">
-        <f>SUM(G11:G12)</f>
+      <c r="H13" s="74"/>
+      <c r="I13" s="87">
+        <f>SUM(I11:I12)</f>
         <v>2</v>
       </c>
-      <c r="H13" s="138">
+      <c r="J13" s="88">
         <v>2</v>
       </c>
-      <c r="I13" s="139"/>
-      <c r="J13" s="139">
+      <c r="K13" s="89"/>
+      <c r="L13" s="89">
         <v>27.5</v>
       </c>
-      <c r="K13" s="140">
-        <f>G13*H13*J13*1000</f>
+      <c r="M13" s="90">
+        <f>I13*J13*L13*1000</f>
         <v>110000</v>
       </c>
-      <c r="L13" s="141">
-        <f>K13*E13</f>
+      <c r="N13" s="91">
+        <f>M13*G13</f>
         <v>220000</v>
       </c>
-      <c r="M13" s="125"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="125"/>
-      <c r="P13" s="129"/>
-      <c r="Q13" s="125"/>
-      <c r="R13" s="129"/>
-      <c r="S13" s="130"/>
-      <c r="T13" s="124"/>
-      <c r="U13" s="125"/>
-      <c r="V13" s="129"/>
-      <c r="W13" s="125"/>
-      <c r="X13" s="129"/>
-      <c r="Y13" s="131"/>
-      <c r="Z13" s="132"/>
-      <c r="AA13" s="133"/>
-      <c r="AB13" s="124"/>
-      <c r="AC13" s="125"/>
-      <c r="AD13" s="129"/>
-      <c r="AE13" s="134"/>
-      <c r="AF13" s="128"/>
-      <c r="AG13" s="134"/>
-      <c r="AH13" s="128"/>
-      <c r="AI13" s="135"/>
-      <c r="AJ13" s="129"/>
-    </row>
-    <row r="14" spans="1:48" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="121"/>
-      <c r="B14" s="122"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="124"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="125"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="124"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="127"/>
-      <c r="L14" s="128"/>
-      <c r="M14" s="125"/>
-      <c r="N14" s="129"/>
-      <c r="O14" s="125"/>
-      <c r="P14" s="129"/>
-      <c r="Q14" s="125"/>
-      <c r="R14" s="129"/>
-      <c r="S14" s="130"/>
-      <c r="T14" s="124"/>
-      <c r="U14" s="125"/>
-      <c r="V14" s="129"/>
-      <c r="W14" s="125"/>
-      <c r="X14" s="129"/>
-      <c r="Y14" s="131"/>
-      <c r="Z14" s="132"/>
-      <c r="AA14" s="133"/>
-      <c r="AB14" s="124"/>
-      <c r="AC14" s="125"/>
-      <c r="AD14" s="129"/>
-      <c r="AE14" s="134"/>
-      <c r="AF14" s="128"/>
-      <c r="AG14" s="134"/>
-      <c r="AH14" s="128"/>
-      <c r="AI14" s="135"/>
-      <c r="AJ14" s="129"/>
-    </row>
-    <row r="15" spans="1:48" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="121">
+      <c r="O13" s="75"/>
+      <c r="P13" s="79"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="79"/>
+      <c r="S13" s="75"/>
+      <c r="T13" s="79"/>
+      <c r="U13" s="80"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="75"/>
+      <c r="X13" s="79"/>
+      <c r="Y13" s="75"/>
+      <c r="Z13" s="79"/>
+      <c r="AA13" s="81"/>
+      <c r="AB13" s="82"/>
+      <c r="AC13" s="83"/>
+      <c r="AD13" s="74"/>
+      <c r="AE13" s="75"/>
+      <c r="AF13" s="79"/>
+      <c r="AG13" s="84"/>
+      <c r="AH13" s="78"/>
+      <c r="AI13" s="84"/>
+      <c r="AJ13" s="78"/>
+      <c r="AK13" s="85"/>
+      <c r="AL13" s="79"/>
+    </row>
+    <row r="14" spans="1:50" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="71"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="167"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="75"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="75"/>
+      <c r="T14" s="79"/>
+      <c r="U14" s="80"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="75"/>
+      <c r="X14" s="79"/>
+      <c r="Y14" s="75"/>
+      <c r="Z14" s="79"/>
+      <c r="AA14" s="81"/>
+      <c r="AB14" s="82"/>
+      <c r="AC14" s="83"/>
+      <c r="AD14" s="74"/>
+      <c r="AE14" s="75"/>
+      <c r="AF14" s="79"/>
+      <c r="AG14" s="84"/>
+      <c r="AH14" s="78"/>
+      <c r="AI14" s="84"/>
+      <c r="AJ14" s="78"/>
+      <c r="AK14" s="85"/>
+      <c r="AL14" s="79"/>
+    </row>
+    <row r="15" spans="1:50" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="71">
         <v>3</v>
       </c>
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="164"/>
+      <c r="C15" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="123"/>
-      <c r="D15" s="124" t="s">
+      <c r="D15" s="73"/>
+      <c r="E15" s="167"/>
+      <c r="F15" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="124">
+      <c r="G15" s="74">
         <v>1</v>
       </c>
-      <c r="F15" s="124">
+      <c r="H15" s="74">
         <v>3</v>
       </c>
-      <c r="G15" s="125">
+      <c r="I15" s="75">
         <v>4</v>
       </c>
-      <c r="H15" s="126">
+      <c r="J15" s="76">
         <v>1.5</v>
       </c>
-      <c r="I15" s="124">
+      <c r="K15" s="74">
         <v>11</v>
       </c>
-      <c r="J15" s="124">
+      <c r="L15" s="74">
         <v>28</v>
       </c>
-      <c r="K15" s="127">
-        <f>J15*H15*G15*1000</f>
+      <c r="M15" s="77">
+        <f>L15*J15*I15*1000</f>
         <v>168000</v>
       </c>
-      <c r="L15" s="128">
-        <f t="shared" ref="L15:L17" si="4">K15*E15</f>
+      <c r="N15" s="78">
+        <f t="shared" ref="N15:N17" si="4">M15*G15</f>
         <v>168000</v>
       </c>
-      <c r="M15" s="125">
+      <c r="O15" s="75">
         <v>480</v>
       </c>
-      <c r="N15" s="129">
-        <f>G15*M15*E15</f>
+      <c r="P15" s="79">
+        <f>I15*O15*G15</f>
         <v>1920</v>
       </c>
-      <c r="O15" s="125">
+      <c r="Q15" s="75">
         <v>480</v>
       </c>
-      <c r="P15" s="129">
-        <f>G15*O15*E15</f>
+      <c r="R15" s="79">
+        <f>I15*Q15*G15</f>
         <v>1920</v>
       </c>
-      <c r="Q15" s="125">
+      <c r="S15" s="75">
         <v>360</v>
       </c>
-      <c r="R15" s="129">
+      <c r="T15" s="79">
         <v>360</v>
       </c>
-      <c r="S15" s="130">
+      <c r="U15" s="80">
         <v>1</v>
       </c>
-      <c r="T15" s="124">
+      <c r="V15" s="74">
         <v>1</v>
       </c>
-      <c r="U15" s="125">
+      <c r="W15" s="75">
         <v>96</v>
       </c>
-      <c r="V15" s="129">
-        <f t="shared" ref="V15:V16" si="5">T15*U15*S15</f>
+      <c r="X15" s="79">
+        <f t="shared" ref="X15:X16" si="5">V15*W15*U15</f>
         <v>96</v>
       </c>
-      <c r="W15" s="125">
+      <c r="Y15" s="75">
         <v>60</v>
       </c>
-      <c r="X15" s="129">
+      <c r="Z15" s="79">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="Y15" s="131">
-        <f t="shared" ref="Y15:Y20" si="6">180*T15</f>
+      <c r="AA15" s="81">
+        <f t="shared" ref="AA15:AA20" si="6">180*V15</f>
         <v>180</v>
       </c>
-      <c r="Z15" s="132">
+      <c r="AB15" s="82">
         <v>180</v>
       </c>
-      <c r="AA15" s="133">
+      <c r="AC15" s="83">
         <v>180</v>
       </c>
-      <c r="AB15" s="124"/>
-      <c r="AC15" s="125">
+      <c r="AD15" s="74"/>
+      <c r="AE15" s="75">
         <v>60</v>
       </c>
-      <c r="AD15" s="129">
-        <f t="shared" ref="AD15:AD20" si="7">AC15*AB15</f>
+      <c r="AF15" s="79">
+        <f t="shared" ref="AF15:AF20" si="7">AE15*AD15</f>
         <v>0</v>
       </c>
-      <c r="AE15" s="134"/>
-      <c r="AF15" s="128">
-        <f>AE15*N15</f>
+      <c r="AG15" s="84"/>
+      <c r="AH15" s="78">
+        <f>AG15*P15</f>
         <v>0</v>
       </c>
-      <c r="AG15" s="134"/>
-      <c r="AH15" s="128">
-        <f>AG15*K15</f>
+      <c r="AI15" s="84"/>
+      <c r="AJ15" s="78">
+        <f>AI15*M15</f>
         <v>0</v>
       </c>
-      <c r="AI15" s="135"/>
-      <c r="AJ15" s="129">
+      <c r="AK15" s="85"/>
+      <c r="AL15" s="79">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:48" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="121">
+    <row r="16" spans="1:50" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="71">
         <v>4</v>
       </c>
-      <c r="B16" s="122" t="s">
+      <c r="B16" s="164"/>
+      <c r="C16" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="D16" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="124"/>
-      <c r="E16" s="124">
+      <c r="E16" s="167"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74">
         <v>1</v>
       </c>
-      <c r="F16" s="124">
+      <c r="H16" s="74">
         <v>4</v>
       </c>
-      <c r="G16" s="125">
+      <c r="I16" s="75">
         <v>4</v>
       </c>
-      <c r="H16" s="126">
+      <c r="J16" s="76">
         <v>1.5</v>
       </c>
-      <c r="I16" s="124">
+      <c r="K16" s="74">
         <v>11</v>
       </c>
-      <c r="J16" s="124">
+      <c r="L16" s="74">
         <v>28</v>
       </c>
-      <c r="K16" s="127">
-        <f>J16*H16*G16*1000</f>
+      <c r="M16" s="77">
+        <f>L16*J16*I16*1000</f>
         <v>168000</v>
       </c>
-      <c r="L16" s="128">
+      <c r="N16" s="78">
         <f t="shared" si="4"/>
         <v>168000</v>
       </c>
-      <c r="M16" s="125">
+      <c r="O16" s="75">
         <v>480</v>
       </c>
-      <c r="N16" s="129">
-        <f>G16*M16*E16</f>
+      <c r="P16" s="79">
+        <f>I16*O16*G16</f>
         <v>1920</v>
       </c>
-      <c r="O16" s="125">
+      <c r="Q16" s="75">
         <v>480</v>
       </c>
-      <c r="P16" s="129">
-        <f>G16*O16*E16</f>
+      <c r="R16" s="79">
+        <f>I16*Q16*G16</f>
         <v>1920</v>
       </c>
-      <c r="Q16" s="125">
+      <c r="S16" s="75">
         <v>360</v>
       </c>
-      <c r="R16" s="129">
+      <c r="T16" s="79">
         <v>360</v>
       </c>
-      <c r="S16" s="130">
+      <c r="U16" s="80">
         <v>1</v>
       </c>
-      <c r="T16" s="124">
+      <c r="V16" s="74">
         <v>1</v>
       </c>
-      <c r="U16" s="125">
+      <c r="W16" s="75">
         <v>96</v>
       </c>
-      <c r="V16" s="129">
+      <c r="X16" s="79">
         <f t="shared" si="5"/>
         <v>96</v>
       </c>
-      <c r="W16" s="125">
+      <c r="Y16" s="75">
         <v>60</v>
       </c>
-      <c r="X16" s="129">
-        <f t="shared" ref="X16:X23" si="8">W16*T16</f>
+      <c r="Z16" s="79">
+        <f t="shared" ref="Z16:Z23" si="8">Y16*V16</f>
         <v>60</v>
       </c>
-      <c r="Y16" s="131">
+      <c r="AA16" s="81">
         <f t="shared" si="6"/>
         <v>180</v>
       </c>
-      <c r="Z16" s="132">
+      <c r="AB16" s="82">
         <v>180</v>
       </c>
-      <c r="AA16" s="133">
+      <c r="AC16" s="83">
         <v>180</v>
       </c>
-      <c r="AB16" s="124"/>
-      <c r="AC16" s="125">
+      <c r="AD16" s="74"/>
+      <c r="AE16" s="75">
         <v>60</v>
       </c>
-      <c r="AD16" s="129">
+      <c r="AF16" s="79">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AE16" s="134"/>
-      <c r="AF16" s="128">
-        <f>AE16*N16</f>
+      <c r="AG16" s="84"/>
+      <c r="AH16" s="78">
+        <f>AG16*P16</f>
         <v>0</v>
       </c>
-      <c r="AG16" s="134"/>
-      <c r="AH16" s="128">
-        <f>AG16*K16</f>
+      <c r="AI16" s="84"/>
+      <c r="AJ16" s="78">
+        <f>AI16*M16</f>
         <v>0</v>
       </c>
-      <c r="AI16" s="135"/>
-      <c r="AJ16" s="129">
+      <c r="AK16" s="85"/>
+      <c r="AL16" s="79">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="121"/>
-      <c r="B17" s="122"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="124"/>
-      <c r="E17" s="124">
+    <row r="17" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="71"/>
+      <c r="B17" s="164"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74">
         <v>1</v>
       </c>
-      <c r="F17" s="124"/>
-      <c r="G17" s="137">
-        <f>SUM(G15:G16)</f>
+      <c r="H17" s="74"/>
+      <c r="I17" s="87">
+        <f>SUM(I15:I16)</f>
         <v>8</v>
       </c>
-      <c r="H17" s="138">
+      <c r="J17" s="88">
         <v>1.5</v>
       </c>
-      <c r="I17" s="139"/>
-      <c r="J17" s="139">
+      <c r="K17" s="89"/>
+      <c r="L17" s="89">
         <v>28</v>
       </c>
-      <c r="K17" s="140">
-        <f>G17*H17*J17*1000</f>
+      <c r="M17" s="90">
+        <f>I17*J17*L17*1000</f>
         <v>336000</v>
       </c>
-      <c r="L17" s="141">
+      <c r="N17" s="91">
         <f t="shared" si="4"/>
         <v>336000</v>
       </c>
-      <c r="M17" s="125"/>
-      <c r="N17" s="129"/>
-      <c r="O17" s="125"/>
-      <c r="P17" s="129"/>
-      <c r="Q17" s="125"/>
-      <c r="R17" s="129"/>
-      <c r="S17" s="130"/>
-      <c r="T17" s="124"/>
-      <c r="U17" s="125"/>
-      <c r="V17" s="129"/>
-      <c r="W17" s="125"/>
-      <c r="X17" s="129"/>
-      <c r="Y17" s="131"/>
-      <c r="Z17" s="132"/>
-      <c r="AA17" s="133"/>
-      <c r="AB17" s="124"/>
-      <c r="AC17" s="125"/>
-      <c r="AD17" s="129"/>
-      <c r="AE17" s="134"/>
-      <c r="AF17" s="128"/>
-      <c r="AG17" s="134"/>
-      <c r="AH17" s="128"/>
-      <c r="AI17" s="135"/>
-      <c r="AJ17" s="129"/>
-    </row>
-    <row r="18" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="121"/>
-      <c r="B18" s="122"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="125"/>
-      <c r="H18" s="126"/>
-      <c r="I18" s="124"/>
-      <c r="J18" s="124"/>
-      <c r="K18" s="127"/>
-      <c r="L18" s="128"/>
-      <c r="M18" s="125"/>
-      <c r="N18" s="129"/>
-      <c r="O18" s="125"/>
-      <c r="P18" s="129"/>
-      <c r="Q18" s="125"/>
-      <c r="R18" s="129"/>
-      <c r="S18" s="130"/>
-      <c r="T18" s="124"/>
-      <c r="U18" s="125"/>
-      <c r="V18" s="129"/>
-      <c r="W18" s="125"/>
-      <c r="X18" s="129"/>
-      <c r="Y18" s="131"/>
-      <c r="Z18" s="132"/>
-      <c r="AA18" s="133"/>
-      <c r="AB18" s="124"/>
-      <c r="AC18" s="125"/>
-      <c r="AD18" s="129"/>
-      <c r="AE18" s="134"/>
-      <c r="AF18" s="128"/>
-      <c r="AG18" s="134"/>
-      <c r="AH18" s="128"/>
-      <c r="AI18" s="135"/>
-      <c r="AJ18" s="129"/>
-    </row>
-    <row r="19" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="121">
+      <c r="O17" s="75"/>
+      <c r="P17" s="79"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="79"/>
+      <c r="S17" s="75"/>
+      <c r="T17" s="79"/>
+      <c r="U17" s="80"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="75"/>
+      <c r="X17" s="79"/>
+      <c r="Y17" s="75"/>
+      <c r="Z17" s="79"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="82"/>
+      <c r="AC17" s="83"/>
+      <c r="AD17" s="74"/>
+      <c r="AE17" s="75"/>
+      <c r="AF17" s="79"/>
+      <c r="AG17" s="84"/>
+      <c r="AH17" s="78"/>
+      <c r="AI17" s="84"/>
+      <c r="AJ17" s="78"/>
+      <c r="AK17" s="85"/>
+      <c r="AL17" s="79"/>
+    </row>
+    <row r="18" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="71"/>
+      <c r="B18" s="164"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="78"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="79"/>
+      <c r="S18" s="75"/>
+      <c r="T18" s="79"/>
+      <c r="U18" s="80"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="75"/>
+      <c r="X18" s="79"/>
+      <c r="Y18" s="75"/>
+      <c r="Z18" s="79"/>
+      <c r="AA18" s="81"/>
+      <c r="AB18" s="82"/>
+      <c r="AC18" s="83"/>
+      <c r="AD18" s="74"/>
+      <c r="AE18" s="75"/>
+      <c r="AF18" s="79"/>
+      <c r="AG18" s="84"/>
+      <c r="AH18" s="78"/>
+      <c r="AI18" s="84"/>
+      <c r="AJ18" s="78"/>
+      <c r="AK18" s="85"/>
+      <c r="AL18" s="79"/>
+    </row>
+    <row r="19" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="71">
         <v>5</v>
       </c>
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="164"/>
+      <c r="C19" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="123"/>
-      <c r="D19" s="124"/>
-      <c r="E19" s="124">
+      <c r="D19" s="73"/>
+      <c r="E19" s="167"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74">
         <v>1</v>
       </c>
-      <c r="F19" s="124">
+      <c r="H19" s="74">
         <v>5</v>
       </c>
-      <c r="G19" s="125">
+      <c r="I19" s="75">
         <v>1</v>
       </c>
-      <c r="H19" s="126">
+      <c r="J19" s="76">
         <v>2</v>
       </c>
-      <c r="I19" s="124">
+      <c r="K19" s="74">
         <v>7</v>
       </c>
-      <c r="J19" s="124">
+      <c r="L19" s="74">
         <v>28</v>
       </c>
-      <c r="K19" s="127">
-        <f>J19*H19*G19*1000</f>
+      <c r="M19" s="77">
+        <f>L19*J19*I19*1000</f>
         <v>56000</v>
       </c>
-      <c r="L19" s="128">
-        <f t="shared" ref="L19:L21" si="9">K19*E19</f>
+      <c r="N19" s="78">
+        <f t="shared" ref="N19:N21" si="9">M19*G19</f>
         <v>56000</v>
       </c>
-      <c r="M19" s="125">
+      <c r="O19" s="75">
         <v>480</v>
       </c>
-      <c r="N19" s="129">
-        <f>G19*M19*E19</f>
+      <c r="P19" s="79">
+        <f>I19*O19*G19</f>
         <v>480</v>
       </c>
-      <c r="O19" s="125">
+      <c r="Q19" s="75">
         <v>480</v>
       </c>
-      <c r="P19" s="129">
-        <f>G19*O19*E19</f>
+      <c r="R19" s="79">
+        <f>I19*Q19*G19</f>
         <v>480</v>
       </c>
-      <c r="Q19" s="125"/>
-      <c r="R19" s="129">
-        <f>G19*Q19</f>
+      <c r="S19" s="75"/>
+      <c r="T19" s="79">
+        <f>I19*S19</f>
         <v>0</v>
       </c>
-      <c r="S19" s="130">
+      <c r="U19" s="80">
         <v>1</v>
       </c>
-      <c r="T19" s="124">
+      <c r="V19" s="74">
         <v>1</v>
       </c>
-      <c r="U19" s="125">
+      <c r="W19" s="75">
         <v>96</v>
       </c>
-      <c r="V19" s="129">
-        <f t="shared" ref="V19:V20" si="10">T19*U19*S19</f>
+      <c r="X19" s="79">
+        <f t="shared" ref="X19:X20" si="10">V19*W19*U19</f>
         <v>96</v>
       </c>
-      <c r="W19" s="125">
+      <c r="Y19" s="75">
         <v>60</v>
       </c>
-      <c r="X19" s="129">
+      <c r="Z19" s="79">
         <f t="shared" si="8"/>
         <v>60</v>
       </c>
-      <c r="Y19" s="131">
+      <c r="AA19" s="81">
         <f t="shared" si="6"/>
         <v>180</v>
       </c>
-      <c r="Z19" s="132">
+      <c r="AB19" s="82">
         <v>180</v>
       </c>
-      <c r="AA19" s="133">
+      <c r="AC19" s="83">
         <v>180</v>
       </c>
-      <c r="AB19" s="124">
+      <c r="AD19" s="74">
         <v>2</v>
       </c>
-      <c r="AC19" s="125">
+      <c r="AE19" s="75">
         <v>60</v>
       </c>
-      <c r="AD19" s="129">
+      <c r="AF19" s="79">
         <f t="shared" si="7"/>
         <v>120</v>
       </c>
-      <c r="AE19" s="134"/>
-      <c r="AF19" s="128">
-        <f>AE19*N19</f>
+      <c r="AG19" s="84"/>
+      <c r="AH19" s="78">
+        <f>AG19*P19</f>
         <v>0</v>
       </c>
-      <c r="AG19" s="134"/>
-      <c r="AH19" s="128">
-        <f>AG19*K19</f>
+      <c r="AI19" s="84"/>
+      <c r="AJ19" s="78">
+        <f>AI19*M19</f>
         <v>0</v>
       </c>
-      <c r="AI19" s="135"/>
-      <c r="AJ19" s="129">
+      <c r="AK19" s="85"/>
+      <c r="AL19" s="79">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="121">
+    <row r="20" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="71">
         <v>6</v>
       </c>
-      <c r="B20" s="122" t="s">
+      <c r="B20" s="164"/>
+      <c r="C20" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="123"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124">
+      <c r="D20" s="73"/>
+      <c r="E20" s="167"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74">
         <v>1</v>
       </c>
-      <c r="F20" s="124">
+      <c r="H20" s="74">
         <v>6</v>
       </c>
-      <c r="G20" s="125">
+      <c r="I20" s="75">
         <v>1</v>
       </c>
-      <c r="H20" s="126">
+      <c r="J20" s="76">
         <v>2</v>
       </c>
-      <c r="I20" s="124">
+      <c r="K20" s="74">
         <v>7</v>
       </c>
-      <c r="J20" s="124">
+      <c r="L20" s="74">
         <v>28</v>
       </c>
-      <c r="K20" s="127">
-        <f>J20*H20*G20*1000</f>
+      <c r="M20" s="77">
+        <f>L20*J20*I20*1000</f>
         <v>56000</v>
       </c>
-      <c r="L20" s="128">
+      <c r="N20" s="78">
         <f t="shared" si="9"/>
         <v>56000</v>
       </c>
-      <c r="M20" s="125">
+      <c r="O20" s="75">
         <v>480</v>
       </c>
-      <c r="N20" s="129">
-        <f>G20*M20*E20</f>
+      <c r="P20" s="79">
+        <f>I20*O20*G20</f>
         <v>480</v>
       </c>
-      <c r="O20" s="125">
+      <c r="Q20" s="75">
         <v>480</v>
       </c>
-      <c r="P20" s="129">
-        <f>G20*O20*E20</f>
+      <c r="R20" s="79">
+        <f>I20*Q20*G20</f>
         <v>480</v>
       </c>
-      <c r="Q20" s="125"/>
-      <c r="R20" s="129">
-        <f>G20*Q20</f>
+      <c r="S20" s="75"/>
+      <c r="T20" s="79">
+        <f>I20*S20</f>
         <v>0</v>
       </c>
-      <c r="S20" s="130">
+      <c r="U20" s="80">
         <v>1</v>
       </c>
-      <c r="T20" s="124">
+      <c r="V20" s="74">
         <v>1</v>
       </c>
-      <c r="U20" s="125">
+      <c r="W20" s="75">
         <v>96</v>
       </c>
-      <c r="V20" s="129">
+      <c r="X20" s="79">
         <f t="shared" si="10"/>
         <v>96</v>
       </c>
-      <c r="W20" s="125">
+      <c r="Y20" s="75">
         <v>60</v>
       </c>
-      <c r="X20" s="129">
+      <c r="Z20" s="79">
         <f t="shared" si="8"/>
         <v>60</v>
       </c>
-      <c r="Y20" s="131">
+      <c r="AA20" s="81">
         <f t="shared" si="6"/>
         <v>180</v>
       </c>
-      <c r="Z20" s="132">
+      <c r="AB20" s="82">
         <v>180</v>
       </c>
-      <c r="AA20" s="133">
+      <c r="AC20" s="83">
         <v>180</v>
       </c>
-      <c r="AB20" s="124">
+      <c r="AD20" s="74">
         <v>2</v>
       </c>
-      <c r="AC20" s="125">
+      <c r="AE20" s="75">
         <v>60</v>
       </c>
-      <c r="AD20" s="129">
+      <c r="AF20" s="79">
         <f t="shared" si="7"/>
         <v>120</v>
       </c>
-      <c r="AE20" s="134"/>
-      <c r="AF20" s="128">
-        <f>AE20*N20</f>
+      <c r="AG20" s="84"/>
+      <c r="AH20" s="78">
+        <f>AG20*P20</f>
         <v>0</v>
       </c>
-      <c r="AG20" s="134"/>
-      <c r="AH20" s="128">
-        <f>AG20*K20</f>
+      <c r="AI20" s="84"/>
+      <c r="AJ20" s="78">
+        <f>AI20*M20</f>
         <v>0</v>
       </c>
-      <c r="AI20" s="135"/>
-      <c r="AJ20" s="129">
+      <c r="AK20" s="85"/>
+      <c r="AL20" s="79">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="121"/>
-      <c r="B21" s="122"/>
-      <c r="C21" s="123"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="124">
+    <row r="21" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="71"/>
+      <c r="B21" s="164"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="167"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74">
         <v>1</v>
       </c>
-      <c r="F21" s="124"/>
-      <c r="G21" s="137">
-        <f>SUM(G19:G20)</f>
+      <c r="H21" s="74"/>
+      <c r="I21" s="87">
+        <f>SUM(I19:I20)</f>
         <v>2</v>
       </c>
-      <c r="H21" s="138">
+      <c r="J21" s="88">
         <v>2</v>
       </c>
-      <c r="I21" s="139"/>
-      <c r="J21" s="139">
+      <c r="K21" s="89"/>
+      <c r="L21" s="89">
         <v>28</v>
       </c>
-      <c r="K21" s="140">
-        <f>G21*H21*J21*1000</f>
+      <c r="M21" s="90">
+        <f>I21*J21*L21*1000</f>
         <v>112000</v>
       </c>
-      <c r="L21" s="141">
+      <c r="N21" s="91">
         <f t="shared" si="9"/>
         <v>112000</v>
       </c>
-      <c r="M21" s="125"/>
-      <c r="N21" s="129"/>
-      <c r="O21" s="125"/>
-      <c r="P21" s="129"/>
-      <c r="Q21" s="125"/>
-      <c r="R21" s="129"/>
-      <c r="S21" s="130"/>
-      <c r="T21" s="124"/>
-      <c r="U21" s="125"/>
-      <c r="V21" s="129"/>
-      <c r="W21" s="125"/>
-      <c r="X21" s="129"/>
-      <c r="Y21" s="131"/>
-      <c r="Z21" s="132"/>
-      <c r="AA21" s="133"/>
-      <c r="AB21" s="124"/>
-      <c r="AC21" s="125"/>
-      <c r="AD21" s="129"/>
-      <c r="AE21" s="134"/>
-      <c r="AF21" s="128"/>
-      <c r="AG21" s="134"/>
-      <c r="AH21" s="128"/>
-      <c r="AI21" s="135"/>
-      <c r="AJ21" s="129"/>
-    </row>
-    <row r="22" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="121"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="124"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="125"/>
-      <c r="H22" s="126"/>
-      <c r="I22" s="124"/>
-      <c r="J22" s="124"/>
-      <c r="K22" s="127"/>
-      <c r="L22" s="128"/>
-      <c r="M22" s="125"/>
-      <c r="N22" s="129"/>
-      <c r="O22" s="125"/>
-      <c r="P22" s="129"/>
-      <c r="Q22" s="125"/>
-      <c r="R22" s="129"/>
-      <c r="S22" s="130"/>
-      <c r="T22" s="124"/>
-      <c r="U22" s="125"/>
-      <c r="V22" s="129"/>
-      <c r="W22" s="125"/>
-      <c r="X22" s="129"/>
-      <c r="Y22" s="131"/>
-      <c r="Z22" s="132"/>
-      <c r="AA22" s="133"/>
-      <c r="AB22" s="124"/>
-      <c r="AC22" s="125"/>
-      <c r="AD22" s="129"/>
-      <c r="AE22" s="134"/>
-      <c r="AF22" s="128"/>
-      <c r="AG22" s="134"/>
-      <c r="AH22" s="128"/>
-      <c r="AI22" s="135"/>
-      <c r="AJ22" s="129"/>
-    </row>
-    <row r="23" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="121">
+      <c r="O21" s="75"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="79"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="79"/>
+      <c r="U21" s="80"/>
+      <c r="V21" s="74"/>
+      <c r="W21" s="75"/>
+      <c r="X21" s="79"/>
+      <c r="Y21" s="75"/>
+      <c r="Z21" s="79"/>
+      <c r="AA21" s="81"/>
+      <c r="AB21" s="82"/>
+      <c r="AC21" s="83"/>
+      <c r="AD21" s="74"/>
+      <c r="AE21" s="75"/>
+      <c r="AF21" s="79"/>
+      <c r="AG21" s="84"/>
+      <c r="AH21" s="78"/>
+      <c r="AI21" s="84"/>
+      <c r="AJ21" s="78"/>
+      <c r="AK21" s="85"/>
+      <c r="AL21" s="79"/>
+    </row>
+    <row r="22" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="71"/>
+      <c r="B22" s="164"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="167"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="77"/>
+      <c r="N22" s="78"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="79"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="79"/>
+      <c r="S22" s="75"/>
+      <c r="T22" s="79"/>
+      <c r="U22" s="80"/>
+      <c r="V22" s="74"/>
+      <c r="W22" s="75"/>
+      <c r="X22" s="79"/>
+      <c r="Y22" s="75"/>
+      <c r="Z22" s="79"/>
+      <c r="AA22" s="81"/>
+      <c r="AB22" s="82"/>
+      <c r="AC22" s="83"/>
+      <c r="AD22" s="74"/>
+      <c r="AE22" s="75"/>
+      <c r="AF22" s="79"/>
+      <c r="AG22" s="84"/>
+      <c r="AH22" s="78"/>
+      <c r="AI22" s="84"/>
+      <c r="AJ22" s="78"/>
+      <c r="AK22" s="85"/>
+      <c r="AL22" s="79"/>
+    </row>
+    <row r="23" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="71">
         <v>7</v>
       </c>
-      <c r="B23" s="122" t="s">
+      <c r="B23" s="164"/>
+      <c r="C23" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C23" s="123"/>
-      <c r="D23" s="124"/>
-      <c r="E23" s="124">
+      <c r="D23" s="73"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74">
         <v>1</v>
       </c>
-      <c r="F23" s="124">
+      <c r="H23" s="74">
         <v>7</v>
       </c>
-      <c r="G23" s="125">
+      <c r="I23" s="75">
         <v>4</v>
       </c>
-      <c r="H23" s="126">
+      <c r="J23" s="76">
         <v>2</v>
       </c>
-      <c r="I23" s="124">
+      <c r="K23" s="74">
         <v>4</v>
       </c>
-      <c r="J23" s="124">
+      <c r="L23" s="74">
         <v>40</v>
       </c>
-      <c r="K23" s="127">
-        <f>J23*H23*G23*1000</f>
+      <c r="M23" s="77">
+        <f>L23*J23*I23*1000</f>
         <v>320000</v>
       </c>
-      <c r="L23" s="128">
-        <f t="shared" ref="L23:L25" si="11">K23*E23</f>
+      <c r="N23" s="78">
+        <f t="shared" ref="N23:N25" si="11">M23*G23</f>
         <v>320000</v>
       </c>
-      <c r="M23" s="125">
+      <c r="O23" s="75">
         <v>480</v>
       </c>
-      <c r="N23" s="129">
-        <f>G23*M23*E23</f>
+      <c r="P23" s="79">
+        <f>I23*O23*G23</f>
         <v>1920</v>
       </c>
-      <c r="O23" s="125">
+      <c r="Q23" s="75">
         <v>480</v>
       </c>
-      <c r="P23" s="129">
-        <f>G23*O23*E23</f>
+      <c r="R23" s="79">
+        <f>I23*Q23*G23</f>
         <v>1920</v>
       </c>
-      <c r="Q23" s="125">
+      <c r="S23" s="75">
         <v>360</v>
       </c>
-      <c r="R23" s="129">
+      <c r="T23" s="79">
         <v>360</v>
       </c>
-      <c r="S23" s="130">
+      <c r="U23" s="80">
         <v>1</v>
       </c>
-      <c r="T23" s="124">
+      <c r="V23" s="74">
         <v>1</v>
       </c>
-      <c r="U23" s="125">
+      <c r="W23" s="75">
         <v>96</v>
       </c>
-      <c r="V23" s="129">
-        <f t="shared" ref="V23:V24" si="12">T23*U23*S23</f>
+      <c r="X23" s="79">
+        <f t="shared" ref="X23:X24" si="12">V23*W23*U23</f>
         <v>96</v>
       </c>
-      <c r="W23" s="125">
+      <c r="Y23" s="75">
         <v>60</v>
       </c>
-      <c r="X23" s="129">
+      <c r="Z23" s="79">
         <f t="shared" si="8"/>
         <v>60</v>
       </c>
-      <c r="Y23" s="131">
-        <f t="shared" ref="Y23:Y24" si="13">180*T23</f>
+      <c r="AA23" s="81">
+        <f t="shared" ref="AA23:AA24" si="13">180*V23</f>
         <v>180</v>
       </c>
-      <c r="Z23" s="132">
+      <c r="AB23" s="82">
         <v>180</v>
       </c>
-      <c r="AA23" s="133">
+      <c r="AC23" s="83">
         <v>180</v>
       </c>
-      <c r="AB23" s="124"/>
-      <c r="AC23" s="125">
+      <c r="AD23" s="74"/>
+      <c r="AE23" s="75">
         <v>60</v>
       </c>
-      <c r="AD23" s="129">
-        <f t="shared" ref="AD23:AD24" si="14">AC23*AB23</f>
+      <c r="AF23" s="79">
+        <f t="shared" ref="AF23:AF24" si="14">AE23*AD23</f>
         <v>0</v>
       </c>
-      <c r="AE23" s="134"/>
-      <c r="AF23" s="128">
-        <f>AE23*N23</f>
+      <c r="AG23" s="84"/>
+      <c r="AH23" s="78">
+        <f>AG23*P23</f>
         <v>0</v>
       </c>
-      <c r="AG23" s="134"/>
-      <c r="AH23" s="128">
-        <f>AG23*K23</f>
+      <c r="AI23" s="84"/>
+      <c r="AJ23" s="78">
+        <f>AI23*M23</f>
         <v>0</v>
       </c>
-      <c r="AI23" s="135"/>
-      <c r="AJ23" s="129">
+      <c r="AK23" s="85"/>
+      <c r="AL23" s="79">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="121">
+    <row r="24" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="71">
         <v>8</v>
       </c>
-      <c r="B24" s="122" t="s">
+      <c r="B24" s="164"/>
+      <c r="C24" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="123"/>
-      <c r="D24" s="124"/>
-      <c r="E24" s="124">
+      <c r="D24" s="73"/>
+      <c r="E24" s="167"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74">
         <v>1</v>
       </c>
-      <c r="F24" s="124">
+      <c r="H24" s="74">
         <v>8</v>
       </c>
-      <c r="G24" s="125">
+      <c r="I24" s="75">
         <v>4</v>
       </c>
-      <c r="H24" s="126">
+      <c r="J24" s="76">
         <v>2</v>
       </c>
-      <c r="I24" s="124">
+      <c r="K24" s="74">
         <v>4</v>
       </c>
-      <c r="J24" s="124">
+      <c r="L24" s="74">
         <v>40</v>
       </c>
-      <c r="K24" s="127">
-        <f>J24*H24*G24*1000</f>
+      <c r="M24" s="77">
+        <f>L24*J24*I24*1000</f>
         <v>320000</v>
       </c>
-      <c r="L24" s="128">
+      <c r="N24" s="78">
         <f t="shared" si="11"/>
         <v>320000</v>
       </c>
-      <c r="M24" s="125">
+      <c r="O24" s="75">
         <v>480</v>
       </c>
-      <c r="N24" s="129">
-        <f>G24*M24*E24</f>
+      <c r="P24" s="79">
+        <f>I24*O24*G24</f>
         <v>1920</v>
       </c>
-      <c r="O24" s="125">
+      <c r="Q24" s="75">
         <v>480</v>
       </c>
-      <c r="P24" s="129">
-        <f>G24*O24*E24</f>
+      <c r="R24" s="79">
+        <f>I24*Q24*G24</f>
         <v>1920</v>
       </c>
-      <c r="Q24" s="125">
+      <c r="S24" s="75">
         <v>360</v>
       </c>
-      <c r="R24" s="129">
+      <c r="T24" s="79">
         <v>360</v>
       </c>
-      <c r="S24" s="130">
+      <c r="U24" s="80">
         <v>1</v>
       </c>
-      <c r="T24" s="124">
+      <c r="V24" s="74">
         <v>1</v>
       </c>
-      <c r="U24" s="125">
+      <c r="W24" s="75">
         <v>96</v>
       </c>
-      <c r="V24" s="129">
+      <c r="X24" s="79">
         <f t="shared" si="12"/>
         <v>96</v>
       </c>
-      <c r="W24" s="125">
+      <c r="Y24" s="75">
         <v>60</v>
       </c>
-      <c r="X24" s="129">
-        <f t="shared" ref="X24" si="15">W24*T24</f>
+      <c r="Z24" s="79">
+        <f t="shared" ref="Z24" si="15">Y24*V24</f>
         <v>60</v>
       </c>
-      <c r="Y24" s="131">
+      <c r="AA24" s="81">
         <f t="shared" si="13"/>
         <v>180</v>
       </c>
-      <c r="Z24" s="132"/>
-      <c r="AA24" s="133"/>
-      <c r="AB24" s="124"/>
-      <c r="AC24" s="125">
+      <c r="AB24" s="82"/>
+      <c r="AC24" s="83"/>
+      <c r="AD24" s="74"/>
+      <c r="AE24" s="75">
         <v>60</v>
       </c>
-      <c r="AD24" s="129">
+      <c r="AF24" s="79">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE24" s="134"/>
-      <c r="AF24" s="128">
-        <f>AE24*N24</f>
+      <c r="AG24" s="84"/>
+      <c r="AH24" s="78">
+        <f>AG24*P24</f>
         <v>0</v>
       </c>
-      <c r="AG24" s="134"/>
-      <c r="AH24" s="128">
-        <f>AG24*K24</f>
+      <c r="AI24" s="84"/>
+      <c r="AJ24" s="78">
+        <f>AI24*M24</f>
         <v>0</v>
       </c>
-      <c r="AI24" s="135"/>
-      <c r="AJ24" s="129">
+      <c r="AK24" s="85"/>
+      <c r="AL24" s="79">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="142"/>
-      <c r="B25" s="143"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="124"/>
-      <c r="E25" s="124">
+    <row r="25" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="92"/>
+      <c r="B25" s="165"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74">
         <v>1</v>
       </c>
-      <c r="F25" s="124">
+      <c r="H25" s="74">
         <v>8</v>
       </c>
-      <c r="G25" s="137">
-        <f>SUM(G23:G24)</f>
+      <c r="I25" s="87">
+        <f>SUM(I23:I24)</f>
         <v>8</v>
       </c>
-      <c r="H25" s="138">
+      <c r="J25" s="88">
         <v>2</v>
       </c>
-      <c r="I25" s="139" t="s">
+      <c r="K25" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="J25" s="139">
+      <c r="L25" s="89">
         <v>40</v>
       </c>
-      <c r="K25" s="140">
-        <f>G25*H25*J25*1000</f>
+      <c r="M25" s="90">
+        <f>I25*J25*L25*1000</f>
         <v>640000</v>
       </c>
-      <c r="L25" s="145">
+      <c r="N25" s="95">
         <f t="shared" si="11"/>
         <v>640000</v>
       </c>
-      <c r="M25" s="125"/>
-      <c r="N25" s="146"/>
-      <c r="O25" s="125"/>
-      <c r="P25" s="129"/>
-      <c r="Q25" s="125"/>
-      <c r="R25" s="129"/>
-      <c r="S25" s="130"/>
-      <c r="T25" s="124"/>
-      <c r="U25" s="125"/>
-      <c r="V25" s="129"/>
-      <c r="W25" s="125"/>
-      <c r="X25" s="129"/>
-      <c r="Y25" s="131"/>
-      <c r="Z25" s="132"/>
-      <c r="AA25" s="133"/>
-      <c r="AB25" s="124"/>
-      <c r="AC25" s="125"/>
-      <c r="AD25" s="129"/>
-      <c r="AE25" s="125"/>
-      <c r="AF25" s="128"/>
-      <c r="AG25" s="125"/>
-      <c r="AH25" s="128"/>
-      <c r="AI25" s="135"/>
-      <c r="AJ25" s="129"/>
-    </row>
-    <row r="26" spans="1:36" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="147"/>
-      <c r="B26" s="148"/>
-      <c r="C26" s="149"/>
-      <c r="D26" s="150"/>
-      <c r="E26" s="150"/>
-      <c r="F26" s="150"/>
-      <c r="G26" s="151"/>
-      <c r="H26" s="152"/>
-      <c r="I26" s="150"/>
-      <c r="J26" s="150"/>
-      <c r="K26" s="153"/>
-      <c r="L26" s="154"/>
-      <c r="M26" s="151"/>
-      <c r="N26" s="155"/>
-      <c r="O26" s="151"/>
-      <c r="P26" s="155"/>
-      <c r="Q26" s="151"/>
-      <c r="R26" s="155"/>
-      <c r="S26" s="156"/>
-      <c r="T26" s="150"/>
-      <c r="U26" s="151"/>
-      <c r="V26" s="155"/>
-      <c r="W26" s="151"/>
-      <c r="X26" s="155"/>
-      <c r="Y26" s="157"/>
-      <c r="Z26" s="158"/>
-      <c r="AA26" s="159"/>
-      <c r="AB26" s="150"/>
-      <c r="AC26" s="151"/>
-      <c r="AD26" s="155"/>
-      <c r="AE26" s="151"/>
-      <c r="AF26" s="154"/>
-      <c r="AG26" s="151"/>
-      <c r="AH26" s="154"/>
-      <c r="AI26" s="160"/>
-      <c r="AJ26" s="155"/>
-    </row>
-    <row r="27" spans="1:36" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O25" s="75"/>
+      <c r="P25" s="96"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="79"/>
+      <c r="S25" s="75"/>
+      <c r="T25" s="79"/>
+      <c r="U25" s="80"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="75"/>
+      <c r="X25" s="79"/>
+      <c r="Y25" s="75"/>
+      <c r="Z25" s="79"/>
+      <c r="AA25" s="81"/>
+      <c r="AB25" s="82"/>
+      <c r="AC25" s="83"/>
+      <c r="AD25" s="74"/>
+      <c r="AE25" s="75"/>
+      <c r="AF25" s="79"/>
+      <c r="AG25" s="75"/>
+      <c r="AH25" s="78"/>
+      <c r="AI25" s="75"/>
+      <c r="AJ25" s="78"/>
+      <c r="AK25" s="85"/>
+      <c r="AL25" s="79"/>
+    </row>
+    <row r="26" spans="1:38" s="86" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="97"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="168"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="101"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="103"/>
+      <c r="N26" s="104"/>
+      <c r="O26" s="101"/>
+      <c r="P26" s="105"/>
+      <c r="Q26" s="101"/>
+      <c r="R26" s="105"/>
+      <c r="S26" s="101"/>
+      <c r="T26" s="105"/>
+      <c r="U26" s="106"/>
+      <c r="V26" s="100"/>
+      <c r="W26" s="101"/>
+      <c r="X26" s="105"/>
+      <c r="Y26" s="101"/>
+      <c r="Z26" s="105"/>
+      <c r="AA26" s="107"/>
+      <c r="AB26" s="108"/>
+      <c r="AC26" s="109"/>
+      <c r="AD26" s="100"/>
+      <c r="AE26" s="101"/>
+      <c r="AF26" s="105"/>
+      <c r="AG26" s="101"/>
+      <c r="AH26" s="104"/>
+      <c r="AI26" s="101"/>
+      <c r="AJ26" s="104"/>
+      <c r="AK26" s="110"/>
+      <c r="AL26" s="105"/>
+    </row>
+    <row r="27" spans="1:38" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
+      <c r="C27" s="4"/>
       <c r="F27" s="31"/>
-      <c r="G27" s="80">
-        <f>L13+L17+L21+L25</f>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="158">
+        <f>N13+N17+N21+N25</f>
         <v>1308000</v>
       </c>
-      <c r="H27" s="81"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="81"/>
-      <c r="K27" s="81"/>
-      <c r="L27" s="82"/>
-      <c r="M27" s="112">
-        <f>SUM(N11:N26)</f>
-        <v>10560</v>
-      </c>
-      <c r="N27" s="113"/>
-      <c r="O27" s="114">
+      <c r="J27" s="159"/>
+      <c r="K27" s="159"/>
+      <c r="L27" s="159"/>
+      <c r="M27" s="159"/>
+      <c r="N27" s="160"/>
+      <c r="O27" s="140">
         <f>SUM(P11:P26)</f>
         <v>10560</v>
       </c>
-      <c r="P27" s="115"/>
-      <c r="Q27" s="114">
+      <c r="P27" s="141"/>
+      <c r="Q27" s="142">
         <f>SUM(R11:R26)</f>
+        <v>10560</v>
+      </c>
+      <c r="R27" s="143"/>
+      <c r="S27" s="142">
+        <f>SUM(T11:T26)</f>
         <v>1440</v>
       </c>
-      <c r="R27" s="115"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="77">
-        <f>SUM(V11:V26)</f>
+      <c r="T27" s="143"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="144">
+        <f>SUM(X11:X26)</f>
         <v>768</v>
       </c>
-      <c r="V27" s="78"/>
-      <c r="W27" s="77">
-        <f>SUM(X11:X26)</f>
+      <c r="X27" s="145"/>
+      <c r="Y27" s="144">
+        <f>SUM(Z11:Z26)</f>
         <v>480</v>
       </c>
-      <c r="X27" s="78"/>
-      <c r="Y27" s="49">
-        <f>SUM(Y11:Y26)</f>
+      <c r="Z27" s="145"/>
+      <c r="AA27" s="49">
+        <f>SUM(AA11:AA26)</f>
         <v>1440</v>
       </c>
-      <c r="Z27" s="50">
-        <f>SUM(Z11:Z26)</f>
+      <c r="AB27" s="50">
+        <f>SUM(AB11:AB26)</f>
         <v>1260</v>
       </c>
-      <c r="AA27" s="56">
-        <f>SUM(AA11:AA26)</f>
+      <c r="AC27" s="56">
+        <f>SUM(AC11:AC26)</f>
         <v>1260</v>
       </c>
-      <c r="AC27" s="77">
-        <f>SUM(AD11:AD26)</f>
+      <c r="AE27" s="144">
+        <f>SUM(AF11:AF26)</f>
         <v>360</v>
       </c>
-      <c r="AD27" s="79"/>
-      <c r="AE27" s="70">
-        <f>SUM(AF11:AF26)</f>
-        <v>0</v>
-      </c>
-      <c r="AF27" s="71"/>
-      <c r="AG27" s="70">
+      <c r="AF27" s="157"/>
+      <c r="AG27" s="154">
         <f>SUM(AH11:AH26)</f>
         <v>0</v>
       </c>
-      <c r="AH27" s="71"/>
-      <c r="AI27" s="61">
-        <f>SUM(AI11:AI26)</f>
+      <c r="AH27" s="155"/>
+      <c r="AI27" s="154">
+        <f>SUM(AJ11:AJ26)</f>
         <v>0</v>
       </c>
-      <c r="AJ27" s="62">
-        <f>SUM(AJ11:AJ26)</f>
+      <c r="AJ27" s="155"/>
+      <c r="AK27" s="61">
+        <f>SUM(AK11:AK26)</f>
+        <v>0</v>
+      </c>
+      <c r="AL27" s="62">
+        <f>SUM(AL11:AL26)</f>
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:36" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
+      <c r="C29" s="4"/>
       <c r="F29" s="29"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="J29" s="34"/>
       <c r="K29" s="26"/>
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
-      <c r="Q29" s="34"/>
-    </row>
-    <row r="30" spans="1:36" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="S29" s="34"/>
+    </row>
+    <row r="30" spans="1:38" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
       <c r="F30" s="30"/>
-      <c r="Q30" s="26"/>
-    </row>
-    <row r="31" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="S30" s="26"/>
+    </row>
+    <row r="31" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="Q31" s="26"/>
-    </row>
-    <row r="32" spans="1:36" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C31" s="4"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="S31" s="26"/>
+    </row>
+    <row r="32" spans="1:38" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4"/>
+      <c r="D32" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
       <c r="F32" s="24"/>
-      <c r="H32" s="73" t="s">
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="J32" s="150" t="s">
         <v>7</v>
       </c>
-      <c r="I32" s="72"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="86">
-        <f>G27</f>
+      <c r="K32" s="151"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="163">
+        <f>I27</f>
         <v>1308000</v>
       </c>
-      <c r="L32" s="86"/>
-      <c r="Q32" s="26"/>
-    </row>
-    <row r="33" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N32" s="163"/>
+      <c r="S32" s="26"/>
+    </row>
+    <row r="33" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
       <c r="F33" s="24"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="57"/>
-      <c r="Q33" s="26"/>
-    </row>
-    <row r="34" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="57"/>
+      <c r="S33" s="26"/>
+    </row>
+    <row r="34" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
+      <c r="C34" s="4"/>
       <c r="F34" s="24"/>
-      <c r="H34" s="73" t="s">
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="J34" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="I34" s="72"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="85">
-        <f>M27</f>
+      <c r="K34" s="151"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="152">
+        <f>O27</f>
         <v>10560</v>
       </c>
-      <c r="L34" s="85"/>
-      <c r="Q34" s="26"/>
-    </row>
-    <row r="35" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N34" s="152"/>
+      <c r="S34" s="26"/>
+    </row>
+    <row r="35" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="H35" s="73" t="s">
+      <c r="C35" s="4"/>
+      <c r="J35" s="150" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="72"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="85">
-        <f>O27</f>
+      <c r="K35" s="151"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="152">
+        <f>Q27</f>
         <v>10560</v>
       </c>
-      <c r="L35" s="85"/>
-      <c r="Q35" s="26"/>
-    </row>
-    <row r="36" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N35" s="152"/>
+      <c r="S35" s="26"/>
+    </row>
+    <row r="36" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
-      <c r="H36" s="73" t="s">
+      <c r="C36" s="4"/>
+      <c r="J36" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="I36" s="73"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="75">
-        <f>Q27</f>
+      <c r="K36" s="150"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="125">
+        <f>S27</f>
         <v>1440</v>
       </c>
-      <c r="L36" s="75"/>
-      <c r="Q36" s="26"/>
-    </row>
-    <row r="37" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N36" s="125"/>
+      <c r="S36" s="26"/>
+    </row>
+    <row r="37" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="72" t="s">
+      <c r="J37" s="151" t="s">
         <v>49</v>
       </c>
-      <c r="I37" s="72"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="75">
-        <f>U27</f>
+      <c r="K37" s="151"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="125">
+        <f>W27</f>
         <v>768</v>
       </c>
-      <c r="L37" s="75"/>
-      <c r="Q37" s="26"/>
-    </row>
-    <row r="38" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N37" s="125"/>
+      <c r="S37" s="26"/>
+    </row>
+    <row r="38" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
-      <c r="H38" s="72" t="s">
+      <c r="C38" s="4"/>
+      <c r="J38" s="151" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="72"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="75">
-        <f>W27</f>
+      <c r="K38" s="151"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="125">
+        <f>Y27</f>
         <v>480</v>
       </c>
-      <c r="L38" s="75"/>
-      <c r="Q38" s="26"/>
-    </row>
-    <row r="39" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N38" s="125"/>
+      <c r="S38" s="26"/>
+    </row>
+    <row r="39" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
-      <c r="H39" s="72" t="s">
+      <c r="C39" s="4"/>
+      <c r="J39" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="I39" s="72"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="75">
-        <f>Y27+Z27</f>
+      <c r="K39" s="151"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="125">
+        <f>AA27+AB27</f>
         <v>2700</v>
       </c>
-      <c r="L39" s="75"/>
-      <c r="Q39" s="26"/>
-    </row>
-    <row r="40" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N39" s="125"/>
+      <c r="S39" s="26"/>
+    </row>
+    <row r="40" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4"/>
+      <c r="D40" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H40" s="72" t="s">
+      <c r="J40" s="151" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="72"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="75">
-        <f>AA27</f>
+      <c r="K40" s="151"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="125">
+        <f>AC27</f>
         <v>1260</v>
       </c>
-      <c r="L40" s="75"/>
-      <c r="Q40" s="26"/>
-    </row>
-    <row r="41" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N40" s="125"/>
+      <c r="S40" s="26"/>
+    </row>
+    <row r="41" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4"/>
+      <c r="D41" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="H41" s="72" t="s">
+      <c r="J41" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="I41" s="72"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="75">
-        <f>AC27</f>
+      <c r="K41" s="151"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="125">
+        <f>AE27</f>
         <v>360</v>
       </c>
-      <c r="L41" s="75"/>
-      <c r="Q41" s="26"/>
-    </row>
-    <row r="42" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N41" s="125"/>
+      <c r="S41" s="26"/>
+    </row>
+    <row r="42" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
-      <c r="H42" s="73" t="s">
+      <c r="C42" s="4"/>
+      <c r="J42" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="I42" s="73"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="75">
-        <f>AI27+AJ27</f>
+      <c r="K42" s="150"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="125">
+        <f>AK27+AL27</f>
         <v>120</v>
       </c>
-      <c r="L42" s="75"/>
-      <c r="Q42" s="26"/>
-    </row>
-    <row r="43" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N42" s="125"/>
+      <c r="S42" s="26"/>
+    </row>
+    <row r="43" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
+      <c r="C43" s="4"/>
       <c r="J43" s="26"/>
-      <c r="K43" s="83">
-        <f>SUM(K34:K42)</f>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="161">
+        <f>SUM(M34:M42)</f>
         <v>28248</v>
       </c>
-      <c r="L43" s="84"/>
-      <c r="Q43" s="26"/>
-    </row>
-    <row r="44" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N43" s="162"/>
+      <c r="S43" s="26"/>
+    </row>
+    <row r="44" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
+      <c r="C44" s="4"/>
       <c r="J44" s="26"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="58"/>
-      <c r="Q44" s="26"/>
-    </row>
-    <row r="45" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="57"/>
+      <c r="N44" s="58"/>
+      <c r="S44" s="26"/>
+    </row>
+    <row r="45" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
-      <c r="H45" s="74" t="s">
+      <c r="C45" s="4"/>
+      <c r="J45" s="156" t="s">
         <v>65</v>
       </c>
-      <c r="I45" s="74"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="58"/>
-      <c r="Q45" s="26"/>
-    </row>
-    <row r="46" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="K45" s="156"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="57"/>
+      <c r="N45" s="58"/>
+      <c r="S45" s="26"/>
+    </row>
+    <row r="46" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
-      <c r="H46" s="72" t="s">
+      <c r="C46" s="4"/>
+      <c r="J46" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="73"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="75">
+      <c r="K46" s="150"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="125">
+        <f>AI27</f>
+        <v>0</v>
+      </c>
+      <c r="N46" s="153"/>
+      <c r="S46" s="26"/>
+    </row>
+    <row r="47" spans="1:19" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="J47" s="151" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" s="150"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="125">
         <f>AG27</f>
         <v>0</v>
       </c>
-      <c r="L46" s="76"/>
-      <c r="Q46" s="26"/>
-    </row>
-    <row r="47" spans="1:17" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="H47" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="I47" s="73"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="75">
-        <f>AE27</f>
-        <v>0</v>
-      </c>
-      <c r="L47" s="76"/>
-      <c r="Q47" s="26"/>
-    </row>
-    <row r="48" spans="1:17" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N47" s="153"/>
+      <c r="S47" s="26"/>
+    </row>
+    <row r="48" spans="1:19" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
+      <c r="C48" s="4"/>
       <c r="J48" s="26"/>
-      <c r="K48" s="59"/>
-      <c r="L48" s="60"/>
-      <c r="Q48" s="26"/>
-    </row>
-    <row r="49" spans="1:20" s="5" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="59"/>
+      <c r="N48" s="60"/>
+      <c r="S48" s="26"/>
+    </row>
+    <row r="49" spans="1:22" s="5" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
-      <c r="H49" s="89" t="s">
+      <c r="C49" s="4"/>
+      <c r="J49" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="I49" s="90"/>
-      <c r="J49" s="38"/>
-      <c r="K49" s="87">
-        <f>K32+K43+L46+L47</f>
+      <c r="K49" s="149"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="146">
+        <f>M32+M43+N46+N47</f>
         <v>1336248</v>
       </c>
-      <c r="L49" s="88"/>
-    </row>
-    <row r="50" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N49" s="147"/>
+    </row>
+    <row r="50" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="4"/>
+      <c r="D50" s="28" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E50" s="28"/>
+    </row>
+    <row r="51" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
-      <c r="B51" s="161" t="s">
+      <c r="B51" s="4"/>
+      <c r="C51" s="112" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="161"/>
-    </row>
-    <row r="52" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D51" s="112"/>
+      <c r="E51" s="111"/>
+    </row>
+    <row r="52" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="4"/>
+      <c r="D52" s="28" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="E52" s="28"/>
+    </row>
+    <row r="53" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
-    </row>
-    <row r="54" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="4"/>
+      <c r="D54" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="J54" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M54" s="5" t="s">
+      <c r="O54" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="T54" s="5" t="s">
+      <c r="V54" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
-    </row>
-    <row r="56" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
-    </row>
-    <row r="57" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
-    </row>
-    <row r="58" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
-    </row>
-    <row r="59" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
-    </row>
-    <row r="60" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
-    </row>
-    <row r="61" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C60" s="4"/>
+    </row>
+    <row r="61" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
-    </row>
-    <row r="62" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C61" s="4"/>
+    </row>
+    <row r="62" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
-    </row>
-    <row r="63" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C62" s="4"/>
+    </row>
+    <row r="63" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
-    </row>
-    <row r="64" spans="1:20" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="1:22" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
-    </row>
-    <row r="65" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
-    </row>
-    <row r="66" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C65" s="4"/>
+    </row>
+    <row r="66" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
-    </row>
-    <row r="67" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C66" s="4"/>
+    </row>
+    <row r="67" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
-    </row>
-    <row r="68" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C67" s="4"/>
+    </row>
+    <row r="68" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
-    </row>
-    <row r="69" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C68" s="4"/>
+    </row>
+    <row r="69" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
-    </row>
-    <row r="70" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C69" s="4"/>
+    </row>
+    <row r="70" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-    </row>
-    <row r="71" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C70" s="4"/>
+    </row>
+    <row r="71" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
-    </row>
-    <row r="72" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C71" s="4"/>
+    </row>
+    <row r="72" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-    </row>
-    <row r="73" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C72" s="4"/>
+    </row>
+    <row r="73" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-    </row>
-    <row r="74" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C73" s="4"/>
+    </row>
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
-    </row>
-    <row r="75" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C74" s="4"/>
+    </row>
+    <row r="75" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
-    </row>
-    <row r="76" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C75" s="4"/>
+    </row>
+    <row r="76" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
-    </row>
-    <row r="77" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C76" s="4"/>
+    </row>
+    <row r="77" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
-    </row>
-    <row r="78" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C77" s="4"/>
+    </row>
+    <row r="78" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
-    </row>
-    <row r="79" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C78" s="4"/>
+    </row>
+    <row r="79" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
-    </row>
-    <row r="80" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C79" s="4"/>
+    </row>
+    <row r="80" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
-    </row>
-    <row r="81" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C80" s="4"/>
+    </row>
+    <row r="81" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
-    </row>
-    <row r="82" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C81" s="4"/>
+    </row>
+    <row r="82" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
-    </row>
-    <row r="83" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C82" s="4"/>
+    </row>
+    <row r="83" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
-    </row>
-    <row r="84" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C83" s="4"/>
+    </row>
+    <row r="84" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
-    </row>
-    <row r="85" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C84" s="4"/>
+    </row>
+    <row r="85" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
-    </row>
-    <row r="86" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C85" s="4"/>
+    </row>
+    <row r="86" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
-    </row>
-    <row r="87" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C86" s="4"/>
+    </row>
+    <row r="87" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
-    </row>
-    <row r="88" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C87" s="4"/>
+    </row>
+    <row r="88" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
-    </row>
-    <row r="89" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C88" s="4"/>
+    </row>
+    <row r="89" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
-    </row>
-    <row r="90" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C89" s="4"/>
+    </row>
+    <row r="90" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
-    </row>
-    <row r="91" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C90" s="4"/>
+    </row>
+    <row r="91" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
-    </row>
-    <row r="92" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C91" s="4"/>
+    </row>
+    <row r="92" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
-    </row>
-    <row r="93" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C92" s="4"/>
+    </row>
+    <row r="93" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
-    </row>
-    <row r="94" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C93" s="4"/>
+    </row>
+    <row r="94" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
-    </row>
-    <row r="95" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
-    </row>
-    <row r="96" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C95" s="4"/>
+    </row>
+    <row r="96" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
-    </row>
-    <row r="97" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C96" s="4"/>
+    </row>
+    <row r="97" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
-    </row>
-    <row r="98" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C97" s="4"/>
+    </row>
+    <row r="98" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
-    </row>
-    <row r="99" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
-    </row>
-    <row r="100" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C99" s="4"/>
+    </row>
+    <row r="100" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
-    </row>
-    <row r="101" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C100" s="4"/>
+    </row>
+    <row r="101" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
-    </row>
-    <row r="102" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C101" s="4"/>
+    </row>
+    <row r="102" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
-    </row>
-    <row r="103" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C102" s="4"/>
+    </row>
+    <row r="103" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
-    </row>
-    <row r="104" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C103" s="4"/>
+    </row>
+    <row r="104" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
-    </row>
-    <row r="105" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C104" s="4"/>
+    </row>
+    <row r="105" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
-    </row>
-    <row r="106" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C105" s="4"/>
+    </row>
+    <row r="106" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
-    </row>
-    <row r="107" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C106" s="4"/>
+    </row>
+    <row r="107" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
-    </row>
-    <row r="108" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C107" s="4"/>
+    </row>
+    <row r="108" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
-    </row>
-    <row r="109" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C108" s="4"/>
+    </row>
+    <row r="109" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
-    </row>
-    <row r="110" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C109" s="4"/>
+    </row>
+    <row r="110" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
-    </row>
-    <row r="111" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C110" s="4"/>
+    </row>
+    <row r="111" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-    </row>
-    <row r="112" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C111" s="4"/>
+    </row>
+    <row r="112" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
-    </row>
-    <row r="113" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C112" s="4"/>
+    </row>
+    <row r="113" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
-    </row>
-    <row r="114" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C113" s="4"/>
+    </row>
+    <row r="114" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
-    </row>
-    <row r="115" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C114" s="4"/>
+    </row>
+    <row r="115" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
-    </row>
-    <row r="116" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C115" s="4"/>
+    </row>
+    <row r="116" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
-    </row>
-    <row r="117" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C116" s="4"/>
+    </row>
+    <row r="117" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
-    </row>
-    <row r="118" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C117" s="4"/>
+    </row>
+    <row r="118" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
-    </row>
-    <row r="119" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C118" s="4"/>
+    </row>
+    <row r="119" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
-    </row>
-    <row r="120" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C119" s="4"/>
+    </row>
+    <row r="120" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
-    </row>
-    <row r="121" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C120" s="4"/>
+    </row>
+    <row r="121" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
-    </row>
-    <row r="122" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C121" s="4"/>
+    </row>
+    <row r="122" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
-    </row>
-    <row r="123" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C122" s="4"/>
+    </row>
+    <row r="123" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
-    </row>
-    <row r="124" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C123" s="4"/>
+    </row>
+    <row r="124" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
-    </row>
-    <row r="125" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C124" s="4"/>
+    </row>
+    <row r="125" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
-    </row>
-    <row r="126" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C125" s="4"/>
+    </row>
+    <row r="126" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
-    </row>
-    <row r="127" spans="1:2" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C126" s="4"/>
+    </row>
+    <row r="127" spans="1:3" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A1:AJ1"/>
-    <mergeCell ref="A3:AJ3"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="AI27:AJ27"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="AE27:AF27"/>
+    <mergeCell ref="AG27:AH27"/>
+    <mergeCell ref="I27:N27"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="I6:T6"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="U6:AA6"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A1:AL1"/>
+    <mergeCell ref="A3:AL3"/>
+    <mergeCell ref="J7:M7"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="AG7:AH7"/>
+    <mergeCell ref="AK7:AL7"/>
+    <mergeCell ref="A2:AL2"/>
+    <mergeCell ref="A4:F4"/>
     <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AG6:AJ6"/>
     <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="A2:AJ2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE6:AH6"/>
-    <mergeCell ref="AG7:AH7"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="G6:R6"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="S6:Y6"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="AG27:AH27"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="AC27:AD27"/>
-    <mergeCell ref="AE27:AF27"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="1.5" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="70" orientation="landscape" r:id="rId1"/>

</xml_diff>